<commit_message>
List of 16 functions.
</commit_message>
<xml_diff>
--- a/Perceptron-AND-Function-23-Feb-2025/NBU-CODE-Perceptron-23-Feb-2025.xlsx
+++ b/Perceptron-AND-Function-23-Feb-2025/NBU-CODE-Perceptron-23-Feb-2025.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Perceptron" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="XOR" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Functions" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="bias" vbProcedure="false">Perceptron!$A$2</definedName>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t xml:space="preserve">INPUT</t>
   </si>
@@ -169,6 +170,63 @@
   </si>
   <si>
     <t xml:space="preserve">^</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or</t>
   </si>
 </sst>
 </file>
@@ -231,7 +289,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +368,12 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -352,7 +416,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -429,15 +493,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -503,7 +579,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -696,11 +772,11 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.12890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="16.12"/>
   </cols>
@@ -735,26 +811,26 @@
       </c>
       <c r="B2" s="5" t="n">
         <f aca="true">RAND()</f>
-        <v>0.452959153807137</v>
+        <v>0.0600697991186021</v>
       </c>
       <c r="C2" s="6" t="n">
         <f aca="false">$A$2*$B$2 + A3*$B$3 + A4*$B$4</f>
-        <v>-0.761703884266158</v>
+        <v>-0.24067017271226</v>
       </c>
       <c r="D2" s="6" t="n">
         <f aca="false">TANH( C2 )</f>
-        <v>-0.642079487607007</v>
+        <v>-0.236128655664459</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>-0.95</v>
       </c>
       <c r="F2" s="8" t="n">
         <f aca="false">ABS( D2-E2 )</f>
-        <v>0.307920512392993</v>
+        <v>0.713871344335541</v>
       </c>
       <c r="H2" s="9" t="n">
         <f aca="false">SUM(F2:F5)</f>
-        <v>3.0690432692998</v>
+        <v>3.3282762504033</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,22 +839,22 @@
       </c>
       <c r="B3" s="5" t="n">
         <f aca="true">RAND()</f>
-        <v>0.589116568153341</v>
+        <v>0.00444232471048774</v>
       </c>
       <c r="C3" s="6" t="n">
         <f aca="false">$A$2*$B$2 + A5*$B$3 + A6*$B$4</f>
-        <v>0.548300712389085</v>
+        <v>0.352369353999537</v>
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">TANH( C3 )</f>
-        <v>0.499245547019933</v>
+        <v>0.338475132183488</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>-0.95</v>
       </c>
       <c r="F3" s="8" t="n">
         <f aca="false">ABS( D3-E3 )</f>
-        <v>1.44924554701993</v>
+        <v>1.28847513218349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,22 +863,22 @@
       </c>
       <c r="B4" s="5" t="n">
         <f aca="true">RAND()</f>
-        <v>0.68947610350276</v>
+        <v>0.312126066690419</v>
       </c>
       <c r="C4" s="6" t="n">
         <f aca="false">$A$2*$B$2 + A7*$B$3 + A8*$B$4</f>
-        <v>0.35761759522519</v>
+        <v>-0.232229755762333</v>
       </c>
       <c r="D4" s="6" t="n">
         <f aca="false">TANH( C4 )</f>
-        <v>0.343113823717529</v>
+        <v>-0.228143123135137</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>-0.95</v>
       </c>
       <c r="F4" s="8" t="n">
         <f aca="false">ABS( D4-E4 )</f>
-        <v>1.29311382371753</v>
+        <v>0.721856876864863</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,18 +887,18 @@
       </c>
       <c r="C5" s="6" t="n">
         <f aca="false">$A$2*$B$2 + A9*$B$3 + A10*$B$4</f>
-        <v>1.66762219188043</v>
+        <v>0.360809770949464</v>
       </c>
       <c r="D5" s="6" t="n">
         <f aca="false">TANH( C5 )</f>
-        <v>0.931236613830652</v>
+        <v>0.345927102980589</v>
       </c>
       <c r="E5" s="11" t="n">
         <v>0.95</v>
       </c>
       <c r="F5" s="8" t="n">
         <f aca="false">ABS( D5-E5 )</f>
-        <v>0.018763386169348</v>
+        <v>0.604072897019411</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,7 +1037,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -972,7 +1048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="20" t="s">
         <v>17</v>
       </c>
@@ -1005,12 +1081,12 @@
       <c r="C4" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="22" t="n">
-        <f aca="false"> INT( NOT( B4 ) )</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="22" t="n">
-        <f aca="false"> INT( NOT( C4 ) )</f>
+      <c r="D4" s="21" t="n">
+        <f aca="false">INT( NOT( B4 ) )</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <f aca="false">INT( NOT( C4 ) )</f>
         <v>1</v>
       </c>
       <c r="F4" s="21" t="n">
@@ -1022,11 +1098,11 @@
         <v>0</v>
       </c>
       <c r="H4" s="21" t="n">
-        <f aca="false"> INT( OR( F4,G4 ) )</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="22" t="n">
-        <f aca="false"> INT( _xlfn.XOR( B4, C4 ) )</f>
+        <f aca="false">INT( OR( F4,G4 ) )</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="21" t="n">
+        <f aca="false">INT( _xlfn.XOR( B4, C4 ) )</f>
         <v>0</v>
       </c>
     </row>
@@ -1037,12 +1113,12 @@
       <c r="C5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="n">
-        <f aca="false"> INT( NOT( B5 ) )</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="22" t="n">
-        <f aca="false"> INT( NOT( C5 ) )</f>
+      <c r="D5" s="21" t="n">
+        <f aca="false">INT( NOT( B5 ) )</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="21" t="n">
+        <f aca="false">INT( NOT( C5 ) )</f>
         <v>0</v>
       </c>
       <c r="F5" s="21" t="n">
@@ -1054,11 +1130,11 @@
         <v>1</v>
       </c>
       <c r="H5" s="21" t="n">
-        <f aca="false"> INT( OR( F5,G5 ) )</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="22" t="n">
-        <f aca="false"> INT( _xlfn.XOR( B5, C5 ) )</f>
+        <f aca="false">INT( OR( F5,G5 ) )</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="21" t="n">
+        <f aca="false">INT( _xlfn.XOR( B5, C5 ) )</f>
         <v>1</v>
       </c>
     </row>
@@ -1069,12 +1145,12 @@
       <c r="C6" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="22" t="n">
-        <f aca="false"> INT( NOT( B6 ) )</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="22" t="n">
-        <f aca="false"> INT( NOT( C6 ) )</f>
+      <c r="D6" s="21" t="n">
+        <f aca="false">INT( NOT( B6 ) )</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <f aca="false">INT( NOT( C6 ) )</f>
         <v>1</v>
       </c>
       <c r="F6" s="21" t="n">
@@ -1086,11 +1162,11 @@
         <v>0</v>
       </c>
       <c r="H6" s="21" t="n">
-        <f aca="false"> INT( OR( F6,G6 ) )</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="22" t="n">
-        <f aca="false"> INT( _xlfn.XOR( B6, C6 ) )</f>
+        <f aca="false">INT( OR( F6,G6 ) )</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="21" t="n">
+        <f aca="false">INT( _xlfn.XOR( B6, C6 ) )</f>
         <v>1</v>
       </c>
     </row>
@@ -1101,12 +1177,12 @@
       <c r="C7" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="n">
-        <f aca="false"> INT( NOT( B7 ) )</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="22" t="n">
-        <f aca="false"> INT( NOT( C7 ) )</f>
+      <c r="D7" s="21" t="n">
+        <f aca="false">INT( NOT( B7 ) )</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="21" t="n">
+        <f aca="false">INT( NOT( C7 ) )</f>
         <v>0</v>
       </c>
       <c r="F7" s="21" t="n">
@@ -1118,13 +1194,343 @@
         <v>0</v>
       </c>
       <c r="H7" s="21" t="n">
-        <f aca="false"> INT( OR( F7,G7 ) )</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="22" t="n">
-        <f aca="false"> INT( _xlfn.XOR( B7, C7 ) )</f>
-        <v>0</v>
-      </c>
+        <f aca="false">INT( OR( F7,G7 ) )</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="21" t="n">
+        <f aca="false">INT( _xlfn.XOR( B7, C7 ) )</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="230" zoomScaleNormal="230" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>